<commit_message>
fix: removed redundant checks and moved inputs
</commit_message>
<xml_diff>
--- a/equity_equation.xlsx
+++ b/equity_equation.xlsx
@@ -30,12 +30,17 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,7 +57,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -461,7 +466,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -481,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -491,7 +496,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -511,7 +516,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>21500000</v>
+        <v>26000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>